<commit_message>
fixed some issues with the data, misnamed PDB and misinterpretation of variant for Phillips
</commit_message>
<xml_diff>
--- a/raw_datasets/SiPMAB_subsetted.xlsx
+++ b/raw_datasets/SiPMAB_subsetted.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\kyroyo\rosetta-antibody-ddgs\raw_datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{72340929-3F26-4876-8FCF-55FF9A895374}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4133A126-A814-45BC-834D-2E7A4F81F951}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19410" windowHeight="13875" xr2:uid="{A85C5181-279B-45D3-A0A7-594BAE5E7357}"/>
   </bookViews>
@@ -391,9 +391,6 @@
     <t>HTRP98ALA</t>
   </si>
   <si>
-    <t>1DJQ</t>
-  </si>
-  <si>
     <t>HTYR53ALA</t>
   </si>
   <si>
@@ -722,6 +719,9 @@
   </si>
   <si>
     <t>#PDB</t>
+  </si>
+  <si>
+    <t>1DQJ</t>
   </si>
 </sst>
 </file>
@@ -1095,8 +1095,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21C3E5D0-74B8-4080-96C4-44CD0EA09EBF}">
   <dimension ref="A1:F232"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="G114" sqref="G114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -1109,336 +1109,336 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C2">
         <v>0.17440931928033621</v>
       </c>
       <c r="D2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C3">
         <v>0.84474380016840556</v>
       </c>
       <c r="D3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C4">
         <v>1.7164540277754874</v>
       </c>
       <c r="D4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C5">
         <v>0.47110926287685473</v>
       </c>
       <c r="D5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C6">
         <v>1.646669793450446</v>
       </c>
       <c r="D6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C7">
         <v>0.14401900666106648</v>
       </c>
       <c r="D7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F7" s="2"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B8" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C8">
         <v>7.8119908881587818E-2</v>
       </c>
       <c r="D8" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F8" s="2"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B9" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C9">
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F9" s="2"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B10" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C10">
         <v>-0.10405899505816585</v>
       </c>
       <c r="D10" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F10" s="2"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B11" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C11">
         <v>0.30661767837257514</v>
       </c>
       <c r="D11" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F11" s="2"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B12" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C12">
         <v>-0.51001467777202514</v>
       </c>
       <c r="D12" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F12" s="2"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B13" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C13">
         <v>3.9630997274873181E-3</v>
       </c>
       <c r="D13" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F13" s="2"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B14" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C14">
         <v>1.9031336244386612</v>
       </c>
       <c r="D14" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F14" s="2"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B15" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C15">
         <v>-0.12824525936474807</v>
       </c>
       <c r="D15" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F15" s="2"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B16" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C16">
         <v>7.8119908881587818E-2</v>
       </c>
       <c r="D16" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F16" s="2"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B17" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C17">
         <v>1.235993120019705</v>
       </c>
       <c r="D17" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F17" s="2"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B18" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C18">
         <v>0.70532462752520075</v>
       </c>
       <c r="D18" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F18" s="2"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B19" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C19">
         <v>0.84503255648814068</v>
@@ -1447,13 +1447,13 @@
         <v>72</v>
       </c>
       <c r="E19" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F19" s="2"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B20" t="s">
         <v>63</v>
@@ -1465,16 +1465,16 @@
         <v>72</v>
       </c>
       <c r="E20" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F20" s="2"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B21" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C21">
         <v>0.79763719616851247</v>
@@ -1483,16 +1483,16 @@
         <v>72</v>
       </c>
       <c r="E21" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F21" s="2"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B22" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C22">
         <v>0.3872067980469911</v>
@@ -1501,13 +1501,13 @@
         <v>72</v>
       </c>
       <c r="E22" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F22" s="2"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B23" t="s">
         <v>86</v>
@@ -1519,13 +1519,13 @@
         <v>72</v>
       </c>
       <c r="E23" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F23" s="2"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B24" t="s">
         <v>85</v>
@@ -1537,13 +1537,13 @@
         <v>72</v>
       </c>
       <c r="E24" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F24" s="2"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B25" t="s">
         <v>40</v>
@@ -1555,13 +1555,13 @@
         <v>72</v>
       </c>
       <c r="E25" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F25" s="2"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B26" t="s">
         <v>38</v>
@@ -1573,13 +1573,13 @@
         <v>72</v>
       </c>
       <c r="E26" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F26" s="2"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B27" t="s">
         <v>83</v>
@@ -1591,13 +1591,13 @@
         <v>72</v>
       </c>
       <c r="E27" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F27" s="2"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B28" t="s">
         <v>81</v>
@@ -1609,16 +1609,16 @@
         <v>72</v>
       </c>
       <c r="E28" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F28" s="2"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B29" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C29">
         <v>0.17829212405926143</v>
@@ -1627,16 +1627,16 @@
         <v>72</v>
       </c>
       <c r="E29" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F29" s="2"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B30" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C30">
         <v>-0.20763301569513182</v>
@@ -1645,16 +1645,16 @@
         <v>72</v>
       </c>
       <c r="E30" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F30" s="2"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B31" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C31">
         <v>1.1077507185855353</v>
@@ -1663,16 +1663,16 @@
         <v>72</v>
       </c>
       <c r="E31" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F31" s="2"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B32" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C32">
         <v>-9.8005385846526849E-2</v>
@@ -1681,16 +1681,16 @@
         <v>72</v>
       </c>
       <c r="E32" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F32" s="2"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B33" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C33">
         <v>3.0701660893696596</v>
@@ -1699,16 +1699,16 @@
         <v>72</v>
       </c>
       <c r="E33" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F33" s="2"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B34" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C34">
         <v>0.95298987239416277</v>
@@ -1717,16 +1717,16 @@
         <v>72</v>
       </c>
       <c r="E34" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F34" s="2"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B35" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C35">
         <v>4</v>
@@ -1735,7 +1735,7 @@
         <v>72</v>
       </c>
       <c r="E35" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>7</v>
@@ -1743,7 +1743,7 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B36" t="s">
         <v>86</v>
@@ -1755,16 +1755,16 @@
         <v>72</v>
       </c>
       <c r="E36" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F36" s="2"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B37" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C37">
         <v>3.1036027731247149</v>
@@ -1773,16 +1773,16 @@
         <v>72</v>
       </c>
       <c r="E37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F37" s="2"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B38" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C38">
         <v>1.2815223308473076</v>
@@ -1791,16 +1791,16 @@
         <v>72</v>
       </c>
       <c r="E38" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F38" s="2"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B39" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C39">
         <v>2.2010456399268374</v>
@@ -1809,16 +1809,16 @@
         <v>72</v>
       </c>
       <c r="E39" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F39" s="2"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B40" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C40">
         <v>3.0391599138844247</v>
@@ -1827,16 +1827,16 @@
         <v>72</v>
       </c>
       <c r="E40" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F40" s="2"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B41" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C41">
         <v>3.126748480862922</v>
@@ -1845,13 +1845,13 @@
         <v>72</v>
       </c>
       <c r="E41" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F41" s="2"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B42" t="s">
         <v>63</v>
@@ -1863,16 +1863,16 @@
         <v>72</v>
       </c>
       <c r="E42" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F42" s="2"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B43" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C43">
         <v>0.52465340326495991</v>
@@ -1881,13 +1881,13 @@
         <v>72</v>
       </c>
       <c r="E43" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F43" s="2"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B44" t="s">
         <v>86</v>
@@ -1899,13 +1899,13 @@
         <v>72</v>
       </c>
       <c r="E44" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F44" s="2"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B45" t="s">
         <v>38</v>
@@ -1917,13 +1917,13 @@
         <v>72</v>
       </c>
       <c r="E45" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F45" s="2"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B46" t="s">
         <v>83</v>
@@ -1935,13 +1935,13 @@
         <v>72</v>
       </c>
       <c r="E46" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F46" s="2"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B47" t="s">
         <v>81</v>
@@ -1953,16 +1953,16 @@
         <v>72</v>
       </c>
       <c r="E47" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F47" s="2"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B48" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C48">
         <v>2.9397999576233351</v>
@@ -1971,16 +1971,16 @@
         <v>72</v>
       </c>
       <c r="E48" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F48" s="2"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B49" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C49">
         <v>1.5862372040043287</v>
@@ -1989,16 +1989,16 @@
         <v>72</v>
       </c>
       <c r="E49" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F49" s="2"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B50" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C50">
         <v>4</v>
@@ -2007,7 +2007,7 @@
         <v>72</v>
       </c>
       <c r="E50" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F50" s="2" t="s">
         <v>7</v>
@@ -2015,10 +2015,10 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B51" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C51">
         <v>1.6542864994610564</v>
@@ -2027,13 +2027,13 @@
         <v>72</v>
       </c>
       <c r="E51" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F51" s="2"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B52" t="s">
         <v>63</v>
@@ -2045,16 +2045,16 @@
         <v>72</v>
       </c>
       <c r="E52" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F52" s="2"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B53" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C53">
         <v>1.7319182816274381</v>
@@ -2063,16 +2063,16 @@
         <v>72</v>
       </c>
       <c r="E53" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F53" s="2"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B54" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C54">
         <v>0.6904205129124108</v>
@@ -2081,13 +2081,13 @@
         <v>72</v>
       </c>
       <c r="E54" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F54" s="2"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B55" t="s">
         <v>86</v>
@@ -2099,13 +2099,13 @@
         <v>72</v>
       </c>
       <c r="E55" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F55" s="2"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B56" t="s">
         <v>85</v>
@@ -2117,13 +2117,13 @@
         <v>72</v>
       </c>
       <c r="E56" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F56" s="2"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B57" t="s">
         <v>40</v>
@@ -2135,13 +2135,13 @@
         <v>72</v>
       </c>
       <c r="E57" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F57" s="2"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B58" t="s">
         <v>38</v>
@@ -2153,13 +2153,13 @@
         <v>72</v>
       </c>
       <c r="E58" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F58" s="2"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B59" t="s">
         <v>83</v>
@@ -2171,13 +2171,13 @@
         <v>72</v>
       </c>
       <c r="E59" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F59" s="2"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B60" t="s">
         <v>81</v>
@@ -2189,16 +2189,16 @@
         <v>72</v>
       </c>
       <c r="E60" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F60" s="2"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B61" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C61">
         <v>1.1657957139039894</v>
@@ -2207,16 +2207,16 @@
         <v>72</v>
       </c>
       <c r="E61" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F61" s="2"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B62" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C62">
         <v>1.6044688332623469</v>
@@ -2225,16 +2225,16 @@
         <v>72</v>
       </c>
       <c r="E62" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F62" s="2"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B63" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C63">
         <v>4.1893794180364106</v>
@@ -2243,16 +2243,16 @@
         <v>72</v>
       </c>
       <c r="E63" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F63" s="2"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B64" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C64">
         <v>1.8791269659798147</v>
@@ -2261,16 +2261,16 @@
         <v>72</v>
       </c>
       <c r="E64" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F64" s="2"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B65" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C65">
         <v>2.7958767596947194</v>
@@ -2279,16 +2279,16 @@
         <v>72</v>
       </c>
       <c r="E65" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F65" s="2"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
+        <v>153</v>
+      </c>
+      <c r="B66" t="s">
         <v>154</v>
-      </c>
-      <c r="B66" t="s">
-        <v>155</v>
       </c>
       <c r="C66">
         <v>2.0151455066930861</v>
@@ -2297,16 +2297,16 @@
         <v>72</v>
       </c>
       <c r="E66" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F66" s="2"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B67" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C67">
         <v>4</v>
@@ -2315,7 +2315,7 @@
         <v>72</v>
       </c>
       <c r="E67" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F67" s="3" t="s">
         <v>7</v>
@@ -2323,10 +2323,10 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B68" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C68">
         <v>1.2000295813738369</v>
@@ -2335,16 +2335,16 @@
         <v>90</v>
       </c>
       <c r="E68" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F68" s="2"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B69" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C69">
         <v>0.49164485723827589</v>
@@ -2353,13 +2353,13 @@
         <v>90</v>
       </c>
       <c r="E69" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F69" s="2"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B70" t="s">
         <v>85</v>
@@ -2371,13 +2371,13 @@
         <v>90</v>
       </c>
       <c r="E70" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F70" s="2"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B71" t="s">
         <v>64</v>
@@ -2389,16 +2389,16 @@
         <v>90</v>
       </c>
       <c r="E71" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F71" s="2"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B72" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C72">
         <v>0.94864116269481435</v>
@@ -2407,16 +2407,16 @@
         <v>90</v>
       </c>
       <c r="E72" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F72" s="2"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B73" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C73">
         <v>3.7228747009164991</v>
@@ -2425,16 +2425,16 @@
         <v>90</v>
       </c>
       <c r="E73" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F73" s="2"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B74" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C74">
         <v>2.6991353256467328</v>
@@ -2443,16 +2443,16 @@
         <v>90</v>
       </c>
       <c r="E74" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F74" s="2"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B75" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C75">
         <v>1.0656040772356121</v>
@@ -2461,13 +2461,13 @@
         <v>90</v>
       </c>
       <c r="E75" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F75" s="2"/>
     </row>
     <row r="76" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B76" t="s">
         <v>64</v>
@@ -2476,232 +2476,232 @@
         <v>5.2167230636599289</v>
       </c>
       <c r="D76" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E76" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F76" s="1"/>
     </row>
     <row r="77" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B77" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C77">
         <v>1.3441523473601134</v>
       </c>
       <c r="D77" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E77" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F77" s="1"/>
     </row>
     <row r="78" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B78" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C78">
         <v>5.7102060604468168</v>
       </c>
       <c r="D78" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E78" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F78" s="1"/>
     </row>
     <row r="79" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B79" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C79">
         <v>5.1098847478897937</v>
       </c>
       <c r="D79" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E79" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F79" s="1"/>
     </row>
     <row r="80" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B80" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C80">
         <v>4.5598613013027318</v>
       </c>
       <c r="D80" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E80" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F80" s="1"/>
     </row>
     <row r="81" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B81" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C81">
         <v>4.3953697167984522</v>
       </c>
       <c r="D81" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E81" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F81" s="1"/>
     </row>
     <row r="82" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B82" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C82">
         <v>2.3560379457987821</v>
       </c>
       <c r="D82" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E82" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F82" s="1"/>
     </row>
     <row r="83" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B83" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C83">
         <v>0.95356170595371559</v>
       </c>
       <c r="D83" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E83" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F83" s="1"/>
     </row>
     <row r="84" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B84" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C84">
         <v>2.7083907267445682</v>
       </c>
       <c r="D84" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E84" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F84" s="1"/>
     </row>
     <row r="85" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B85" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C85">
         <v>1.4024762398450665</v>
       </c>
       <c r="D85" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E85" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F85" s="1"/>
     </row>
     <row r="86" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B86" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C86">
         <v>0.17044621955284711</v>
       </c>
       <c r="D86" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E86" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F86" s="1"/>
     </row>
     <row r="87" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B87" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C87">
         <v>1.8991705247111756</v>
       </c>
       <c r="D87" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E87" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F87" s="1"/>
     </row>
     <row r="88" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B88" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C88">
         <v>0.17044621955284711</v>
       </c>
       <c r="D88" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E88" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F88" s="1"/>
     </row>
     <row r="89" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B89" t="s">
         <v>102</v>
@@ -2710,34 +2710,34 @@
         <v>6.0380764105214073</v>
       </c>
       <c r="D89" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E89" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F89" s="1"/>
     </row>
     <row r="90" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B90" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C90">
         <v>7.3231999501436755</v>
       </c>
       <c r="D90" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E90" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F90" s="1"/>
     </row>
     <row r="91" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B91" t="s">
         <v>116</v>
@@ -2746,37 +2746,37 @@
         <v>5.5134230072564474</v>
       </c>
       <c r="D91" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E91" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F91" s="1"/>
     </row>
     <row r="92" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B92" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C92">
         <v>3.2471755269853038</v>
       </c>
       <c r="D92" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E92" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F92" s="1"/>
     </row>
     <row r="93" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B93" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C93">
         <v>0.70646680733384137</v>
@@ -2785,16 +2785,16 @@
         <v>90</v>
       </c>
       <c r="E93" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F93" s="1"/>
     </row>
     <row r="94" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B94" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C94">
         <v>0.62026040371738311</v>
@@ -2803,16 +2803,16 @@
         <v>90</v>
       </c>
       <c r="E94" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F94" s="1"/>
     </row>
     <row r="95" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B95" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C95">
         <v>0.80710305434586083</v>
@@ -2821,16 +2821,16 @@
         <v>90</v>
       </c>
       <c r="E95" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F95" s="1"/>
     </row>
     <row r="96" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A96" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B96" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C96">
         <v>3.2520892859373429</v>
@@ -2839,16 +2839,16 @@
         <v>90</v>
       </c>
       <c r="E96" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F96" s="1"/>
     </row>
     <row r="97" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A97" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B97" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C97">
         <v>1.7498775639640218</v>
@@ -2857,16 +2857,16 @@
         <v>90</v>
       </c>
       <c r="E97" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F97" s="1"/>
     </row>
     <row r="98" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A98" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B98" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C98">
         <v>1.0708415808043679</v>
@@ -2875,16 +2875,16 @@
         <v>90</v>
       </c>
       <c r="E98" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F98" s="1"/>
     </row>
     <row r="99" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A99" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B99" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C99">
         <v>2.0073771728282246</v>
@@ -2893,16 +2893,16 @@
         <v>90</v>
       </c>
       <c r="E99" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F99" s="1"/>
     </row>
     <row r="100" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A100" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B100" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C100">
         <v>1.6102362942692796</v>
@@ -2911,16 +2911,16 @@
         <v>90</v>
       </c>
       <c r="E100" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F100" s="1"/>
     </row>
     <row r="101" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A101" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B101" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C101">
         <v>2.8505909405780248</v>
@@ -2929,16 +2929,16 @@
         <v>90</v>
       </c>
       <c r="E101" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F101" s="1"/>
     </row>
     <row r="102" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A102" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B102" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C102">
         <v>0.36276079485318036</v>
@@ -2947,16 +2947,16 @@
         <v>90</v>
       </c>
       <c r="E102" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F102" s="1"/>
     </row>
     <row r="103" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A103" t="s">
+        <v>125</v>
+      </c>
+      <c r="B103" t="s">
         <v>126</v>
-      </c>
-      <c r="B103" t="s">
-        <v>127</v>
       </c>
       <c r="C103">
         <v>1.5144129929000201</v>
@@ -2965,13 +2965,13 @@
         <v>90</v>
       </c>
       <c r="E103" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F103" s="1"/>
     </row>
     <row r="104" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A104" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B104" t="s">
         <v>78</v>
@@ -2983,13 +2983,13 @@
         <v>90</v>
       </c>
       <c r="E104" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F104" s="1"/>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>117</v>
+        <v>227</v>
       </c>
       <c r="B105" t="s">
         <v>64</v>
@@ -3007,10 +3007,10 @@
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>117</v>
+        <v>227</v>
       </c>
       <c r="B106" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C106">
         <v>4.0927151381533653</v>
@@ -3025,10 +3025,10 @@
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>117</v>
+        <v>227</v>
       </c>
       <c r="B107" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C107">
         <v>2.6810529592618533</v>
@@ -3043,10 +3043,10 @@
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>117</v>
+        <v>227</v>
       </c>
       <c r="B108" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C108">
         <v>1.4340226137094962</v>
@@ -3061,10 +3061,10 @@
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>117</v>
+        <v>227</v>
       </c>
       <c r="B109" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C109">
         <v>1.1350826629072923</v>
@@ -3079,10 +3079,10 @@
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>117</v>
+        <v>227</v>
       </c>
       <c r="B110" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C110">
         <v>2.0151455066930843</v>
@@ -3097,7 +3097,7 @@
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>117</v>
+        <v>227</v>
       </c>
       <c r="B111" t="s">
         <v>102</v>
@@ -3115,10 +3115,10 @@
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>117</v>
+        <v>227</v>
       </c>
       <c r="B112" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C112">
         <v>6.8909761312473181</v>
@@ -3133,10 +3133,10 @@
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
+        <v>227</v>
+      </c>
+      <c r="B113" t="s">
         <v>117</v>
-      </c>
-      <c r="B113" t="s">
-        <v>118</v>
       </c>
       <c r="C113">
         <v>1.1815756198031355</v>
@@ -3151,7 +3151,7 @@
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>117</v>
+        <v>227</v>
       </c>
       <c r="B114" t="s">
         <v>116</v>

</xml_diff>